<commit_message>
category_id in import product
</commit_message>
<xml_diff>
--- a/public/templates/product_template.xlsx
+++ b/public/templates/product_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andru\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C9261D-F0EB-4D37-A0F4-E059D8BAAA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ED125E-EF0F-4B87-BA3F-95ABFAD24D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>images1.jpg, images2.jpg</t>
+  </si>
+  <si>
+    <t>category_id</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,9 +440,10 @@
     <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,8 +459,11 @@
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -471,6 +478,9 @@
       </c>
       <c r="E2" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>